<commit_message>
Java+Spring [Shopping Mall] (Payment ,& Tranjaction Process for AOP)
</commit_message>
<xml_diff>
--- a/FashionShop/src/산출물/쇼핑몰DB.xlsx
+++ b/FashionShop/src/산출물/쇼핑몰DB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\spring_workspace\FashionShop\src\산출물\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\korea_workspace\FashionShop\src\산출물\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1866A020-7A1F-4657-AB4C-5EDE91EE85C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595A18D9-43D7-446F-A48B-7D08C206EF8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{239C4E1C-79D8-481D-A521-AFBDBCCFDCE3}"/>
+    <workbookView xWindow="-20610" yWindow="1695" windowWidth="20730" windowHeight="11760" xr2:uid="{239C4E1C-79D8-481D-A521-AFBDBCCFDCE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="110">
   <si>
     <t>topcategory</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -248,10 +248,223 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>변경 가능성이 있는건 컬럼으로 추가하면 안됌</t>
-  </si>
-  <si>
-    <t>(ex) 이미지1,이미지2,이미지3 컬럼에서 한개 더 늘리라고 명령들어와서 이미지4 까지 늘리는 경우)</t>
+    <t>2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>email_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>email_server</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zipcode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송받을사람</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>누가?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB넣을필요없다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실제 결제할 금액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결제액? 물건가액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지불액(포인트 차감)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우리집</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>receive_addr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>card</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문 요약 (order_summary )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>order_summary_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송정보 ( receiver )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>receiver_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결제방법 ( paymethod )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paymetho_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>order_detail_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total_pay</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total_price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>언제?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>orderdate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연락처</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>order_state</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>order_state_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>state</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문완료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품준비중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송출발</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송완료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paymethod</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paymethod_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>핸드폰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>온라인입금</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가상계좌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선택한 결제방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구매시점의가격price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>receiver_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>receiver_phone</t>
   </si>
 </sst>
 </file>
@@ -295,7 +508,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -366,13 +579,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -418,6 +649,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -427,10 +682,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -747,67 +999,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C318EA7-A007-4846-948D-C1AF8CF010C3}">
-  <dimension ref="B1:S37"/>
+  <dimension ref="B3:S68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.19921875" customWidth="1"/>
-    <col min="6" max="6" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.69921875" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="10" max="10" width="15.59765625" customWidth="1"/>
-    <col min="11" max="11" width="14.09765625" customWidth="1"/>
-    <col min="12" max="12" width="13.09765625" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="16.875" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="17.75" customWidth="1"/>
+    <col min="7" max="7" width="13.75" customWidth="1"/>
+    <col min="8" max="8" width="20.625" customWidth="1"/>
+    <col min="9" max="9" width="21.125" customWidth="1"/>
+    <col min="10" max="10" width="15.625" customWidth="1"/>
+    <col min="11" max="11" width="14.125" customWidth="1"/>
+    <col min="12" max="12" width="13.125" customWidth="1"/>
+    <col min="15" max="15" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="F2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-      <c r="F3" s="18" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
+      <c r="F3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="J3" s="15" t="s">
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="J3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="17"/>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5" t="s">
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15" t="s">
         <v>26</v>
       </c>
       <c r="M4" s="1" t="s">
@@ -819,12 +1064,12 @@
       <c r="O4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="16"/>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -861,11 +1106,11 @@
       <c r="O5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P5" s="19" t="s">
+      <c r="P5" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>1</v>
       </c>
@@ -896,8 +1141,11 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="P6" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>2</v>
       </c>
@@ -928,8 +1176,9 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>3</v>
       </c>
@@ -960,8 +1209,9 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>4</v>
       </c>
@@ -992,8 +1242,9 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
       <c r="F10" s="1">
         <v>5</v>
       </c>
@@ -1015,8 +1266,9 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
       <c r="F11" s="1">
         <v>6</v>
       </c>
@@ -1038,13 +1290,14 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B12" s="15" t="s">
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B12" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="25"/>
       <c r="F12" s="1">
         <v>7</v>
       </c>
@@ -1066,8 +1319,9 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
@@ -1098,8 +1352,9 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>1</v>
       </c>
@@ -1130,17 +1385,12 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B15" s="1">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1">
-        <v>4</v>
-      </c>
-      <c r="D15" s="1">
-        <v>3</v>
-      </c>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
       <c r="F15" s="1">
         <v>10</v>
       </c>
@@ -1162,17 +1412,12 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B16" s="1">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1">
-        <v>4</v>
-      </c>
-      <c r="D16" s="1">
-        <v>4</v>
-      </c>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
       <c r="F16" s="1">
         <v>11</v>
       </c>
@@ -1194,17 +1439,12 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B17" s="1">
-        <v>4</v>
-      </c>
-      <c r="C17" s="1">
-        <v>4</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
       <c r="F17" s="1">
         <v>12</v>
       </c>
@@ -1226,8 +1466,9 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1252,8 +1493,9 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F19" s="1">
         <v>14</v>
       </c>
@@ -1275,8 +1517,9 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F20" s="1">
         <v>15</v>
       </c>
@@ -1298,8 +1541,9 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F21" s="1">
         <v>16</v>
       </c>
@@ -1321,20 +1565,21 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B23" s="18" t="s">
+      <c r="P21" s="1"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B23" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="F23" s="18" t="s">
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="F23" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
@@ -1343,10 +1588,13 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>39</v>
       </c>
@@ -1363,10 +1611,13 @@
         <v>30</v>
       </c>
       <c r="H25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
         <v>1</v>
       </c>
@@ -1383,10 +1634,13 @@
         <v>4</v>
       </c>
       <c r="H26" s="1">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
         <v>2</v>
       </c>
@@ -1403,10 +1657,13 @@
         <v>4</v>
       </c>
       <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28" s="1">
         <v>3</v>
       </c>
@@ -1419,8 +1676,9 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B29" s="1">
         <v>4</v>
       </c>
@@ -1434,19 +1692,19 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B31" s="15" t="s">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B31" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="17"/>
-      <c r="F31" s="15" t="s">
+      <c r="C31" s="24"/>
+      <c r="D31" s="25"/>
+      <c r="F31" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="G31" s="16"/>
-      <c r="H31" s="17"/>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="G31" s="24"/>
+      <c r="H31" s="25"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
       <c r="D32" s="9" t="s">
@@ -1458,7 +1716,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
         <v>42</v>
       </c>
@@ -1478,7 +1736,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="1">
         <v>1</v>
       </c>
@@ -1489,16 +1747,16 @@
         <v>32</v>
       </c>
       <c r="F34" s="1">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="G34" s="1">
         <v>4</v>
       </c>
-      <c r="H34" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="H34" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="1">
         <v>2</v>
       </c>
@@ -1514,11 +1772,11 @@
       <c r="G35" s="1">
         <v>4</v>
       </c>
-      <c r="H35" s="1">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="H35" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="1">
         <v>3</v>
       </c>
@@ -1534,11 +1792,11 @@
       <c r="G36" s="1">
         <v>4</v>
       </c>
-      <c r="H36" s="1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="H36" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" s="1">
         <v>4</v>
       </c>
@@ -1554,12 +1812,324 @@
       <c r="G37" s="1">
         <v>4</v>
       </c>
-      <c r="H37" s="1">
-        <v>38</v>
+      <c r="H37" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40" t="s">
+        <v>63</v>
+      </c>
+      <c r="G40" t="s">
+        <v>64</v>
+      </c>
+      <c r="H40" t="s">
+        <v>65</v>
+      </c>
+      <c r="I40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B42" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="20"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B44" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B45" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B46" s="1">
+        <v>23</v>
+      </c>
+      <c r="C46" s="1">
+        <v>5</v>
+      </c>
+      <c r="D46" s="1">
+        <v>50000</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="26">
+        <v>44204</v>
+      </c>
+      <c r="G46" s="1">
+        <v>2</v>
+      </c>
+      <c r="H46" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B49" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="20"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B50" s="2"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B51" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B52" s="1"/>
+      <c r="C52" s="1">
+        <v>23</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B55" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="25"/>
+      <c r="E55" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="20"/>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B56" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J56" s="3"/>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E57" s="1">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1">
+        <v>23</v>
+      </c>
+      <c r="G57" s="1">
+        <v>5</v>
+      </c>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B58" s="1"/>
+      <c r="C58" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E58" s="1">
+        <v>2</v>
+      </c>
+      <c r="F58" s="1">
+        <v>23</v>
+      </c>
+      <c r="G58" s="3">
+        <v>6</v>
+      </c>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B59" s="1"/>
+      <c r="C59" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B60" s="1"/>
+      <c r="C60" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B63" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C63" s="25"/>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B64" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B65" s="1">
+        <v>1</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B66" s="1">
+        <v>2</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B67" s="1">
+        <v>3</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B68" s="1">
+        <v>4</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="13">
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="E55:J55"/>
     <mergeCell ref="J3:O3"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B3:D3"/>
@@ -1568,23 +2138,63 @@
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="F3:H3"/>
+    <mergeCell ref="B55:C55"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8112E76-C31D-45EE-BF06-10F217007FB4}">
-  <dimension ref="A1"/>
+  <dimension ref="F8:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15:O27"/>
+      <selection activeCell="G14" sqref="G14:J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="8" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+    </row>
+    <row r="14" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="G14" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+    </row>
+    <row r="15" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1">
+        <v>23</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J16" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G14:J14"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>